<commit_message>
Moved things around to clean up function argument lists.
</commit_message>
<xml_diff>
--- a/n-Puzzle/Heuristic.xlsx
+++ b/n-Puzzle/Heuristic.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\Git Projects\n-Puzzle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\Git Projects\n-Puzzle\n-Puzzle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3925B70F-87D0-4F72-9EBA-1F2019770946}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F422E8-AFD0-47FC-A72C-36E773D29680}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15270" windowHeight="4410" xr2:uid="{0BF03B89-E9D9-459A-8757-6D954397165E}"/>
   </bookViews>
@@ -394,23 +394,23 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B1">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F1">
         <v>1</v>
@@ -430,16 +430,16 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>12</v>
       </c>
       <c r="D2">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F2">
         <v>5</v>
@@ -459,13 +459,13 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C3">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D3">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="F3">
         <v>9</v>
@@ -484,21 +484,21 @@
       </c>
       <c r="L3">
         <f>SUM(C16:F19)</f>
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F4">
         <v>13</v>
@@ -526,17 +526,17 @@
       </c>
       <c r="L5">
         <f>L3 + 2 * L4</f>
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>IF(A1 = 0, -1, IF(MOD(A1, $K$1) = 0, 3, MOD(A1, $K$1) - 1))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B6">
         <f t="shared" ref="B6:D6" si="0">IF(B1 = 0, -1, IF(MOD(B1, $K$1) = 0, 3, MOD(B1, $K$1) - 1))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
@@ -544,7 +544,7 @@
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="F6">
         <f t="shared" ref="F6:H8" si="1">IF(F1 = 0, -1, IF(MOD(F1, $K$1) = 0, 3, MOD(F1, $K$1) - 1))</f>
@@ -566,11 +566,11 @@
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ref="A7:D7" si="3">IF(A2 = 0, -1, IF(MOD(A2, $K$1) = 0, 3, MOD(A2, $K$1) - 1))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B7">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <f t="shared" si="3"/>
@@ -578,7 +578,7 @@
       </c>
       <c r="D7">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
@@ -604,7 +604,7 @@
       </c>
       <c r="B8">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <f t="shared" si="4"/>
@@ -612,7 +612,7 @@
       </c>
       <c r="D8">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
@@ -634,15 +634,15 @@
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" ref="A9:D9" si="5">IF(A4 = 0, -1, IF(MOD(A4, $K$1) = 0, 3, MOD(A4, $K$1) - 1))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B9">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D9">
         <f t="shared" si="5"/>
@@ -668,19 +668,19 @@
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>IF(A1 = 0, -1, IF(MOD(A1, $K$1) = 0, TRUNC(A1 / $K$1, 0) - 1, TRUNC(A1 / $K$1, 0)))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B11">
         <f t="shared" ref="B11:D11" si="7">IF(B1 = 0, -1, IF(MOD(B1, $K$1) = 0, TRUNC(B1 / $K$1, 0) - 1, TRUNC(B1 / $K$1, 0)))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C11">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F11">
         <f t="shared" ref="F11:H13" si="8">IF(F1 = 0, -1, IF(MOD(F1, $K$1) = 0, TRUNC(F1 / $K$1, 0) - 1, TRUNC(F1 / $K$1, 0)))</f>
@@ -702,11 +702,11 @@
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" ref="A12:D12" si="10">IF(A2 = 0, -1, IF(MOD(A2, $K$1) = 0, TRUNC(A2 / $K$1, 0) - 1, TRUNC(A2 / $K$1, 0)))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B12">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12">
         <f t="shared" si="10"/>
@@ -740,15 +740,15 @@
       </c>
       <c r="B13">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C13">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D13">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F13">
         <f t="shared" si="8"/>
@@ -778,11 +778,11 @@
       </c>
       <c r="C14">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14">
         <f t="shared" ref="F14:H14" si="13">IF(F4 = 0, -1, IF(MOD(F4, $K$1) = 0, TRUNC(F4 / $K$1, 0) - 1, TRUNC(F4 / $K$1, 0)))</f>
@@ -804,15 +804,15 @@
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C16">
         <f>IF(A6 + A11 = -2, 0, ABS(A6-F6)+ABS(A11-F11))</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D16">
         <f t="shared" ref="D16:F16" si="14">IF(B6 + B11 = -2, 0, ABS(B6-G6)+ABS(B11-G11))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E16">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F16">
         <f t="shared" si="14"/>
@@ -822,11 +822,11 @@
     <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17">
         <f t="shared" ref="C17:C19" si="15">IF(A7 + A12 = -2, 0, ABS(A7-F7)+ABS(A12-F12))</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D17">
         <f t="shared" ref="D17:D19" si="16">IF(B7 + B12 = -2, 0, ABS(B7-G7)+ABS(B12-G12))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E17">
         <f t="shared" ref="E17:E19" si="17">IF(C7 + C12 = -2, 0, ABS(C7-H7)+ABS(C12-H12))</f>
@@ -834,7 +834,7 @@
       </c>
       <c r="F17">
         <f t="shared" ref="F17:F18" si="18">IF(D7 + D12 = -2, 0, ABS(D7-I7)+ABS(D12-I12))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
@@ -844,25 +844,25 @@
       </c>
       <c r="D18">
         <f t="shared" si="16"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E18">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F18">
         <f t="shared" si="18"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C19">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D19">
         <f t="shared" si="16"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E19">
         <f t="shared" si="17"/>
@@ -870,7 +870,7 @@
       </c>
       <c r="F19">
         <f>IF(D9 + D14 = -2, 0,IF(I9 - I14 = -2, 0, ABS(D9-I9)+ABS(D14-I14)))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -891,19 +891,19 @@
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1">
         <f>Manhattan!A1</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B1">
         <f>Manhattan!B1</f>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C1">
         <f>Manhattan!C1</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D1">
         <f>Manhattan!D1</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F1">
         <f>Manhattan!F1</f>
@@ -929,11 +929,11 @@
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>Manhattan!A2</f>
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <f>Manhattan!B2</f>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <f>Manhattan!C2</f>
@@ -941,7 +941,7 @@
       </c>
       <c r="D2">
         <f>Manhattan!D2</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F2">
         <f>Manhattan!F2</f>
@@ -967,15 +967,15 @@
       </c>
       <c r="B3">
         <f>Manhattan!B3</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C3">
         <f>Manhattan!C3</f>
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D3">
         <f>Manhattan!D3</f>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="F3">
         <f>Manhattan!F3</f>
@@ -997,19 +997,19 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>Manhattan!A4</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <f>Manhattan!B4</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <f>Manhattan!C4</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4">
         <f>Manhattan!D4</f>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F4">
         <f>Manhattan!F4</f>
@@ -1059,7 +1059,7 @@
       </c>
       <c r="I6">
         <f>IF(Manhattan!D6 = Manhattan!I6, 1, 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1081,7 +1081,7 @@
       </c>
       <c r="F7">
         <f>IF(Manhattan!A7 = Manhattan!F7, 1, 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7">
         <f>IF(Manhattan!B7 = Manhattan!G7, 1, 0)</f>
@@ -1093,7 +1093,7 @@
       </c>
       <c r="I7">
         <f>IF(Manhattan!D7 = Manhattan!I7, 1, 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1145,11 +1145,11 @@
       </c>
       <c r="F9">
         <f>IF(Manhattan!A9 = Manhattan!F9, 1, 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9">
         <f>IF(Manhattan!B9 = Manhattan!G9, 1, 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9">
         <f>IF(Manhattan!C9 = Manhattan!H9, 1, 0)</f>
@@ -1178,19 +1178,19 @@
       </c>
       <c r="F11">
         <f>IF(Manhattan!A11 = Manhattan!F11, 1, 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11">
         <f>IF(Manhattan!B11 = Manhattan!G11, 1, 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11">
         <f>IF(Manhattan!C11 = Manhattan!H11, 1, 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11">
         <f>IF(Manhattan!D11 = Manhattan!I11, 1, 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1215,7 +1215,7 @@
       </c>
       <c r="G12">
         <f>IF(Manhattan!B12 = Manhattan!G12, 1, 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12">
         <f>IF(Manhattan!C12 = Manhattan!H12, 1, 0)</f>
@@ -1248,15 +1248,15 @@
       </c>
       <c r="G13">
         <f>IF(Manhattan!B13 = Manhattan!G13, 1, 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13">
         <f>IF(Manhattan!C13 = Manhattan!H13, 1, 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13">
         <f>IF(Manhattan!D13 = Manhattan!I13, 1, 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Rearranged functions into and within Npuzzle namespace. Fixed solvable(). AI now solves all possible board configurations and rejects all non-solvable ones.
</commit_message>
<xml_diff>
--- a/n-Puzzle/Heuristic.xlsx
+++ b/n-Puzzle/Heuristic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\Git Projects\n-Puzzle\n-Puzzle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F422E8-AFD0-47FC-A72C-36E773D29680}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CEF9EA0-DD17-4AD1-A17C-7D9749567194}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15270" windowHeight="4410" xr2:uid="{0BF03B89-E9D9-459A-8757-6D954397165E}"/>
   </bookViews>
@@ -394,23 +394,23 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B1">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F1">
         <v>1</v>
@@ -430,16 +430,16 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
         <v>12</v>
-      </c>
-      <c r="D2">
-        <v>10</v>
       </c>
       <c r="F2">
         <v>5</v>
@@ -459,13 +459,13 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>3</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="F3">
         <v>9</v>
@@ -484,21 +484,21 @@
       </c>
       <c r="L3">
         <f>SUM(C16:F19)</f>
-        <v>41</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D4">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F4">
         <v>13</v>
@@ -517,7 +517,7 @@
       </c>
       <c r="L4">
         <f>Linear!D16</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -526,25 +526,25 @@
       </c>
       <c r="L5">
         <f>L3 + 2 * L4</f>
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>IF(A1 = 0, -1, IF(MOD(A1, $K$1) = 0, 3, MOD(A1, $K$1) - 1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6">
         <f t="shared" ref="B6:D6" si="0">IF(B1 = 0, -1, IF(MOD(B1, $K$1) = 0, 3, MOD(B1, $K$1) - 1))</f>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="F6">
         <f t="shared" ref="F6:H8" si="1">IF(F1 = 0, -1, IF(MOD(F1, $K$1) = 0, 3, MOD(F1, $K$1) - 1))</f>
@@ -566,11 +566,11 @@
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ref="A7:D7" si="3">IF(A2 = 0, -1, IF(MOD(A2, $K$1) = 0, 3, MOD(A2, $K$1) - 1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <f t="shared" si="3"/>
@@ -578,7 +578,7 @@
       </c>
       <c r="D7">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
@@ -604,7 +604,7 @@
       </c>
       <c r="B8">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <f t="shared" si="4"/>
@@ -612,7 +612,7 @@
       </c>
       <c r="D8">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
@@ -634,7 +634,7 @@
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" ref="A9:D9" si="5">IF(A4 = 0, -1, IF(MOD(A4, $K$1) = 0, 3, MOD(A4, $K$1) - 1))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B9">
         <f t="shared" si="5"/>
@@ -642,7 +642,7 @@
       </c>
       <c r="C9">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D9">
         <f t="shared" si="5"/>
@@ -668,11 +668,11 @@
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>IF(A1 = 0, -1, IF(MOD(A1, $K$1) = 0, TRUNC(A1 / $K$1, 0) - 1, TRUNC(A1 / $K$1, 0)))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B11">
         <f t="shared" ref="B11:D11" si="7">IF(B1 = 0, -1, IF(MOD(B1, $K$1) = 0, TRUNC(B1 / $K$1, 0) - 1, TRUNC(B1 / $K$1, 0)))</f>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="C11">
         <f t="shared" si="7"/>
@@ -680,7 +680,7 @@
       </c>
       <c r="D11">
         <f t="shared" si="7"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F11">
         <f t="shared" ref="F11:H13" si="8">IF(F1 = 0, -1, IF(MOD(F1, $K$1) = 0, TRUNC(F1 / $K$1, 0) - 1, TRUNC(F1 / $K$1, 0)))</f>
@@ -702,15 +702,15 @@
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" ref="A12:D12" si="10">IF(A2 = 0, -1, IF(MOD(A2, $K$1) = 0, TRUNC(A2 / $K$1, 0) - 1, TRUNC(A2 / $K$1, 0)))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B12">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D12">
         <f t="shared" si="10"/>
@@ -748,7 +748,7 @@
       </c>
       <c r="D13">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F13">
         <f t="shared" si="8"/>
@@ -774,15 +774,15 @@
       </c>
       <c r="B14">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D14">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F14">
         <f t="shared" ref="F14:H14" si="13">IF(F4 = 0, -1, IF(MOD(F4, $K$1) = 0, TRUNC(F4 / $K$1, 0) - 1, TRUNC(F4 / $K$1, 0)))</f>
@@ -804,19 +804,19 @@
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C16">
         <f>IF(A6 + A11 = -2, 0, ABS(A6-F6)+ABS(A11-F11))</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D16">
         <f t="shared" ref="D16:F16" si="14">IF(B6 + B11 = -2, 0, ABS(B6-G6)+ABS(B11-G11))</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E16">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F16">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.25">
@@ -834,7 +834,7 @@
       </c>
       <c r="F17">
         <f t="shared" ref="F17:F18" si="18">IF(D7 + D12 = -2, 0, ABS(D7-I7)+ABS(D12-I12))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
@@ -844,7 +844,7 @@
       </c>
       <c r="D18">
         <f t="shared" si="16"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E18">
         <f t="shared" si="17"/>
@@ -852,25 +852,25 @@
       </c>
       <c r="F18">
         <f t="shared" si="18"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C19">
         <f t="shared" si="15"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D19">
         <f t="shared" si="16"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E19">
         <f t="shared" si="17"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F19">
         <f>IF(D9 + D14 = -2, 0,IF(I9 - I14 = -2, 0, ABS(D9-I9)+ABS(D14-I14)))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -891,19 +891,19 @@
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1">
         <f>Manhattan!A1</f>
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B1">
         <f>Manhattan!B1</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C1">
         <f>Manhattan!C1</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1">
         <f>Manhattan!D1</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F1">
         <f>Manhattan!F1</f>
@@ -929,19 +929,19 @@
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>Manhattan!A2</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <f>Manhattan!B2</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <f>Manhattan!C2</f>
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D2">
         <f>Manhattan!D2</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F2">
         <f>Manhattan!F2</f>
@@ -967,7 +967,7 @@
       </c>
       <c r="B3">
         <f>Manhattan!B3</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <f>Manhattan!C3</f>
@@ -975,7 +975,7 @@
       </c>
       <c r="D3">
         <f>Manhattan!D3</f>
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="F3">
         <f>Manhattan!F3</f>
@@ -997,19 +997,19 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>Manhattan!A4</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <f>Manhattan!B4</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <f>Manhattan!C4</f>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D4">
         <f>Manhattan!D4</f>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F4">
         <f>Manhattan!F4</f>
@@ -1047,7 +1047,7 @@
       </c>
       <c r="F6">
         <f>IF(Manhattan!A6 = Manhattan!F6, 1, 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6">
         <f>IF(Manhattan!B6 = Manhattan!G6, 1, 0)</f>
@@ -1081,11 +1081,11 @@
       </c>
       <c r="F7">
         <f>IF(Manhattan!A7 = Manhattan!F7, 1, 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <f>IF(Manhattan!B7 = Manhattan!G7, 1, 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7">
         <f>IF(Manhattan!C7 = Manhattan!H7, 1, 0)</f>
@@ -1093,7 +1093,7 @@
       </c>
       <c r="I7">
         <f>IF(Manhattan!D7 = Manhattan!I7, 1, 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1103,7 +1103,7 @@
       </c>
       <c r="B8">
         <f t="shared" ref="B8:D8" si="2">IF(G8 = 1, IF(AND(G9 = 1, 0 = MOD(ABS(B3 - B4), $K$1), B4 &lt; B3), 1, 0), 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <f t="shared" si="2"/>
@@ -1119,7 +1119,7 @@
       </c>
       <c r="G8">
         <f>IF(Manhattan!B8 = Manhattan!G8, 1, 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8">
         <f>IF(Manhattan!C8 = Manhattan!H8, 1, 0)</f>
@@ -1178,7 +1178,7 @@
       </c>
       <c r="F11">
         <f>IF(Manhattan!A11 = Manhattan!F11, 1, 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11">
         <f>IF(Manhattan!B11 = Manhattan!G11, 1, 0)</f>
@@ -1211,11 +1211,11 @@
       </c>
       <c r="F12">
         <f>IF(Manhattan!A12 = Manhattan!F12, 1, 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12">
         <f>IF(Manhattan!B12 = Manhattan!G12, 1, 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12">
         <f>IF(Manhattan!C12 = Manhattan!H12, 1, 0)</f>
@@ -1289,13 +1289,13 @@
       </c>
       <c r="I14">
         <f>IF(Manhattan!D14 = Manhattan!I14, 1, 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D16">
         <f>SUM(A6:D9, A11:D14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>